<commit_message>
made plots with week 1 data
</commit_message>
<xml_diff>
--- a/data/Exercise1/Field Exercise 1 Datasheet.xlsx
+++ b/data/Exercise1/Field Exercise 1 Datasheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10710"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8b33585034dea40/Desktop/MODS/Data Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{9E84F72B-4418-42F7-8E30-596E55E63D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F964C94-CFF0-4D10-A770-7F71FCBAE896}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{9E84F72B-4418-42F7-8E30-596E55E63D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7925A1B5-1359-7842-A24D-F1D1FA1EE794}"/>
   <bookViews>
     <workbookView xWindow="1416" yWindow="1848" windowWidth="21624" windowHeight="11112" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,17 @@
     <sheet name="Clinometer_Calculations" sheetId="2" r:id="rId2"/>
     <sheet name="Field_Source" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>American beech (Fagus grandifolia)</t>
   </si>
@@ -458,6 +461,18 @@
   </si>
   <si>
     <t>* Please note that the values for DBHs should be an average of two measurements taken at 90 degrees from each other.</t>
+  </si>
+  <si>
+    <t>eastern white pine (Pinus strobus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>black birch (Betula lenta)</t>
+  </si>
+  <si>
+    <t>red oak (Quercus rubra)</t>
   </si>
 </sst>
 </file>
@@ -815,22 +830,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="5" width="23.19921875" style="1" customWidth="1"/>
-    <col min="6" max="9" width="10.796875" style="1"/>
-    <col min="10" max="10" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.796875" style="1"/>
+    <col min="1" max="1" width="12.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.9609375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="23.1796875" style="1" customWidth="1"/>
+    <col min="6" max="9" width="10.8515625" style="1"/>
+    <col min="10" max="10" width="12.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.76171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.8515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -850,123 +865,273 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2">
+        <v>37.200000000000003</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2">
+        <v>35.6</v>
+      </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="1">
+        <v>25.65</v>
+      </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2">
+        <v>24.92</v>
+      </c>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2">
+        <v>33</v>
+      </c>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2">
+        <v>31</v>
+      </c>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2">
+        <v>40</v>
+      </c>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2">
+        <v>41</v>
+      </c>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="2">
+        <v>38.1</v>
+      </c>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2">
+        <v>19</v>
+      </c>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2">
+        <v>16.399999999999999</v>
+      </c>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -974,7 +1139,7 @@
       <c r="E17" s="2"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -982,7 +1147,7 @@
       <c r="E18" s="2"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -990,7 +1155,7 @@
       <c r="E19" s="2"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -998,7 +1163,7 @@
       <c r="E20" s="2"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1006,7 +1171,7 @@
       <c r="E21" s="2"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1014,7 +1179,7 @@
       <c r="E22" s="2"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1022,7 +1187,7 @@
       <c r="E23" s="2"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1030,7 +1195,7 @@
       <c r="E24" s="2"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1038,7 +1203,7 @@
       <c r="E25" s="2"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1046,7 +1211,7 @@
       <c r="E26" s="2"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1054,7 +1219,7 @@
       <c r="E27" s="2"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1062,7 +1227,7 @@
       <c r="E28" s="2"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1070,35 +1235,35 @@
       <c r="E29" s="2"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1151,21 +1316,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300DFBB1-6D5F-9948-8FF8-9D94378BCAAC}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.9609375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.94921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.48046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1185,34 +1350,64 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="2">
+        <v>17.8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>150</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
       <c r="F2" s="2">
         <f>((D2-E2)/100)*C2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>24.919999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
+      <c r="C3" s="1">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1">
+        <v>140</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F49" si="0">((D3-E3)/100)*C3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+        <v>25.650000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14</v>
+      </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16.239999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="F5" s="2">
@@ -1220,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="F6" s="2">
@@ -1228,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="F7" s="2">
@@ -1236,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="F8" s="2">
@@ -1244,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="F9" s="2">
@@ -1252,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="F10" s="2">
@@ -1260,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="F11" s="2">
@@ -1268,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="F12" s="2">
@@ -1276,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="F13" s="2">
@@ -1284,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="F14" s="2">
@@ -1292,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="F15" s="2">
@@ -1300,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="F16" s="2">
@@ -1308,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="F17" s="2">
@@ -1316,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="F18" s="2">
@@ -1324,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="F19" s="2">
@@ -1332,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="F20" s="2">
@@ -1340,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="F21" s="2">
@@ -1348,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="F22" s="2">
@@ -1356,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="F23" s="2">
@@ -1364,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="F24" s="2">
@@ -1372,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="F25" s="2">
@@ -1380,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="F26" s="2">
@@ -1388,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="F27" s="2">
@@ -1396,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="F28" s="2">
@@ -1404,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="F29" s="2">
@@ -1412,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="F30" s="2">
@@ -1420,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="F31" s="2">
@@ -1428,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="F32" s="2">
@@ -1436,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="F33" s="2">
@@ -1444,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="F34" s="2">
@@ -1452,91 +1647,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F36" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F37" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F38" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F39" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F40" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F41" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F42" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F43" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F44" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F45" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F46" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F47" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F48" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F49" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1569,17 +1764,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08788DF0-D467-1047-AB0E-8B4817892689}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.76171875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1593,7 +1788,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1607,7 +1802,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1621,7 +1816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1632,7 +1827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1643,7 +1838,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1654,15 +1849,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1670,7 +1868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1678,7 +1876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1686,7 +1884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1694,7 +1892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1702,7 +1900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1710,7 +1908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1718,7 +1916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1726,7 +1924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1734,7 +1932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1742,7 +1940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1750,7 +1948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1758,7 +1956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1766,7 +1964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1774,7 +1972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1782,7 +1980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1790,7 +1988,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1798,7 +1996,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1806,7 +2004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1814,7 +2012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1822,7 +2020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1830,7 +2028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>

</xml_diff>